<commit_message>
Updates to exported results
</commit_message>
<xml_diff>
--- a/N6004_fatigue_weld_stress.xlsx
+++ b/N6004_fatigue_weld_stress.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,40 +440,45 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Thickness</t>
+          <t>Designed Thickness</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Leg size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Weld type</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Weld length</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Max σ_eq stress</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>τ_y</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>τ_x</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>τ_wf_max</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>σ_wf</t>
         </is>
@@ -498,27 +503,30 @@
       <c r="D2" t="n">
         <v>0.005</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
+      <c r="E2" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.2497462660245774</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>159741.25</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.016642435546875</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>-0.01947905078125</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.2372957920199091</v>
       </c>
     </row>
@@ -541,27 +549,30 @@
       <c r="D3" t="n">
         <v>0.005</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="E3" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.2566571101262003</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>170254.453125</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.00636875146484375</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.0144463603515625</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.2467330638207104</v>
       </c>
     </row>
@@ -584,27 +595,30 @@
       <c r="D4" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.4002394345873443</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>-78318.484375</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.0145652236328125</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.1587000625</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.368885745827492</v>
       </c>
     </row>
@@ -627,27 +641,30 @@
       <c r="D5" t="n">
         <v>0.004</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
+      <c r="E5" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.1760739819740548</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>112168.2734375</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>-0.008740749023437499</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>-0.0949998203125</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0.005888345404101936</v>
       </c>
     </row>
@@ -670,27 +687,30 @@
       <c r="D6" t="n">
         <v>0.005</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
+      <c r="E6" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>25.62847628089928</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>16424499</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>1.6354675</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>-1.9595315</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>24.38689789482822</v>
       </c>
     </row>
@@ -713,27 +733,30 @@
       <c r="D7" t="n">
         <v>0.005</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
+      <c r="E7" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>25.70168240859466</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>17057958</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.5488408124999999</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>1.49679575</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>24.69215267991813</v>
       </c>
     </row>
@@ -756,27 +779,30 @@
       <c r="D8" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>35.77236311861481</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>-6969863</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>1.25721325</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>14.207979</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>32.95466982768883</v>
       </c>
     </row>
@@ -799,27 +825,30 @@
       <c r="D9" t="n">
         <v>0.004</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
+      <c r="E9" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>15.68002934358307</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>9993825</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>-0.786987125</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>-8.447346999999999</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0.5565892741046112</v>
       </c>
     </row>
@@ -842,27 +871,30 @@
       <c r="D10" t="n">
         <v>0.005</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
+      <c r="E10" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.6707385168869381</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>429282.46875</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>0.04398576953125</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>-0.05193719140625</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0.6376088605232266</v>
       </c>
     </row>
@@ -885,27 +917,30 @@
       <c r="D11" t="n">
         <v>0.005</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
+      <c r="E11" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0.683559360616148</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>453483.375</v>
       </c>
-      <c r="I11" t="n">
-        <v>0.0161203515625</v>
-      </c>
       <c r="J11" t="n">
+        <v>0.0161203525390625</v>
+      </c>
+      <c r="K11" t="n">
         <v>0.0389500546875</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0.656965809938043</v>
       </c>
     </row>
@@ -928,27 +963,30 @@
       <c r="D12" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>1.026333705425261</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>-200621.34375</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>0.03695456640625</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>0.40718971875</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>0.9458009842029732</v>
       </c>
     </row>
@@ -971,27 +1009,30 @@
       <c r="D13" t="n">
         <v>0.004</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
+      <c r="E13" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>0.4509786264015581</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>287310.03125</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>-0.022476125</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>-0.2432025625</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0.01537313883074574</v>
       </c>
     </row>
@@ -1014,27 +1055,30 @@
       <c r="D14" t="n">
         <v>0.005</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
+      <c r="E14" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>1.363593020455186</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>873072</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>0.08851846875</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>-0.1050809921875</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>1.296635172551398</v>
       </c>
     </row>
@@ -1057,27 +1101,30 @@
       <c r="D15" t="n">
         <v>0.005</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
+      <c r="E15" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>1.382171242333603</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>917011.125</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>0.03150816796875</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>0.0793946953125</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>1.328177653833482</v>
       </c>
     </row>
@@ -1100,27 +1147,30 @@
       <c r="D16" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>2.023226485147401</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>-395193.625</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.07232063281249999</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.80302875</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>1.864283348196185</v>
       </c>
     </row>
@@ -1143,27 +1193,30 @@
       <c r="D17" t="n">
         <v>0.004</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
+      <c r="E17" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.8882999846821965</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>565940.625</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>-0.0443858046875</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>-0.47887415625</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0.03067218655768232</v>
       </c>
     </row>
@@ -1186,27 +1239,30 @@
       <c r="D18" t="n">
         <v>0.005</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
+      <c r="E18" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>2.15649551108877</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>1381003</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.1393596875</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>-0.16581653125</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>2.050917609307055</v>
       </c>
     </row>
@@ -1229,27 +1285,30 @@
       <c r="D19" t="n">
         <v>0.005</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
+      <c r="E19" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>2.180448701314343</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>1446681.625</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>0.0489043671875</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>0.1256999765625</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>2.095138571379234</v>
       </c>
     </row>
@@ -1272,27 +1331,30 @@
       <c r="D20" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E20" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F20" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>3.15396693574791</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>-615827.75</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>0.112339796875</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>1.252066125</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>2.906054111603019</v>
       </c>
     </row>
@@ -1315,27 +1377,30 @@
       <c r="D21" t="n">
         <v>0.004</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
+      <c r="E21" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>1.384216549698444</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>881913.4375</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>-0.0692504765625</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>-0.7460954375</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>0.04809138078008658</v>
       </c>
     </row>
@@ -1358,27 +1423,30 @@
       <c r="D22" t="n">
         <v>0.005</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
+      <c r="E22" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>3.610327318962922</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>2312505</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>0.23220540625</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>-0.27690565625</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>3.434230684925028</v>
       </c>
     </row>
@@ -1401,27 +1469,30 @@
       <c r="D23" t="n">
         <v>0.005</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
+      <c r="E23" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>3.640308956807281</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>2415366.5</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>0.08012605468749999</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>0.210673015625</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>3.497705054640551</v>
       </c>
     </row>
@@ -1444,27 +1515,30 @@
       <c r="D24" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E24" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F24" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>5.195324827208863</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>-1013952.75</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>0.18429075</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>2.062896</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>4.786689781315909</v>
       </c>
     </row>
@@ -1487,27 +1561,30 @@
       <c r="D25" t="n">
         <v>0.004</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
+      <c r="E25" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>2.279119340454204</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>1452126.875</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>-0.1141797109375</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>-1.228220125</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>0.07974431871185268</v>
       </c>
     </row>
@@ -1530,27 +1607,30 @@
       <c r="D26" t="n">
         <v>0.005</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
+      <c r="E26" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>5.84365568732855</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>3743622.25</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>0.37452075</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>-0.4474</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>5.559413136749282</v>
       </c>
     </row>
@@ -1573,27 +1653,30 @@
       <c r="D27" t="n">
         <v>0.005</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
+      <c r="E27" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>5.879833697907301</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>3901470.5</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>0.1276096875</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>0.34124625</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>5.649272886260457</v>
       </c>
     </row>
@@ -1616,27 +1699,30 @@
       <c r="D28" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E28" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F28" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>8.306340657008304</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>-1620477.375</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>0.29368590625</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>3.2987005</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>7.652676898137027</v>
       </c>
     </row>
@@ -1659,27 +1745,30 @@
       <c r="D29" t="n">
         <v>0.004</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
+      <c r="E29" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>3.642644925696789</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>2320989.25</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>-0.182675875</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>-1.962748125</v>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>0.1281501584450642</v>
       </c>
     </row>
@@ -1702,27 +1791,30 @@
       <c r="D30" t="n">
         <v>0.005</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
+      <c r="E30" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>8.195559674903006</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>5250876</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>0.52419225</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>-0.626846</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>7.797562004012056</v>
       </c>
     </row>
@@ -1745,27 +1837,30 @@
       <c r="D31" t="n">
         <v>0.005</v>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
+      <c r="E31" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>8.235942837089206</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>5465024</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>0.17730328125</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>0.478774625</v>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>7.912793810599768</v>
       </c>
     </row>
@@ -1788,27 +1883,30 @@
       <c r="D32" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E32" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F32" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>11.56430475514478</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>-2255439.75</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>0.40805215625</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>4.5929455</v>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>10.65396371741739</v>
       </c>
     </row>
@@ -1831,27 +1929,30 @@
       <c r="D33" t="n">
         <v>0.004</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
+      <c r="E33" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>5.07035877448377</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>3230817</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>-0.254415578125</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>-2.73180875</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>0.1789657302131223</v>
       </c>
     </row>
@@ -1874,27 +1975,30 @@
       <c r="D34" t="n">
         <v>0.005</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
+      <c r="E34" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>10.68930013279266</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>6849136.5</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>0.6828180625</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>-0.8171089374999999</v>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>10.17075854720444</v>
       </c>
     </row>
@@ -1917,27 +2021,30 @@
       <c r="D35" t="n">
         <v>0.005</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
+      <c r="E35" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>10.73294082246506</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>7122164</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>0.22988215625</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>0.6245805624999999</v>
       </c>
-      <c r="K35" t="n">
+      <c r="L35" t="n">
         <v>10.31164705239626</v>
       </c>
     </row>
@@ -1960,27 +2067,30 @@
       <c r="D36" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E36" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F36" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>15.01014360433654</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>-2926839.75</v>
       </c>
-      <c r="I36" t="n">
+      <c r="J36" t="n">
         <v>0.528895125</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>5.961828499999999</v>
       </c>
-      <c r="K36" t="n">
+      <c r="L36" t="n">
         <v>13.8282852257274</v>
       </c>
     </row>
@@ -2003,27 +2113,30 @@
       <c r="D37" t="n">
         <v>0.004</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
+      <c r="E37" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>6.580309304143503</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>4193118.75</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
         <v>-0.3302908125</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>-3.54515325</v>
       </c>
-      <c r="K37" t="n">
+      <c r="L37" t="n">
         <v>0.2327827403822939</v>
       </c>
     </row>
@@ -2046,27 +2159,30 @@
       <c r="D38" t="n">
         <v>0.005</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
+      <c r="E38" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
         <v>0.5330616740578963</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>15.79973885641231</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>10124428</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>1.0085714375</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>-1.20765575</v>
       </c>
-      <c r="K38" t="n">
+      <c r="L38" t="n">
         <v>15.03383872534291</v>
       </c>
     </row>
@@ -2089,27 +2205,30 @@
       <c r="D39" t="n">
         <v>0.005</v>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
+      <c r="E39" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>15.85466256336123</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>10521452</v>
       </c>
-      <c r="I39" t="n">
+      <c r="J39" t="n">
         <v>0.33875315625</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>0.9230974375</v>
       </c>
-      <c r="K39" t="n">
+      <c r="L39" t="n">
         <v>15.23213985194267</v>
       </c>
     </row>
@@ -2132,27 +2251,30 @@
       <c r="D40" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E40" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F40" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>0.5705138782188672</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>22.11583387697711</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>-4311116.5</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>0.7783421874999999</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>8.784177</v>
       </c>
-      <c r="K40" t="n">
+      <c r="L40" t="n">
         <v>20.37419252618646</v>
       </c>
     </row>
@@ -2175,27 +2297,30 @@
       <c r="D41" t="n">
         <v>0.004</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
+      <c r="E41" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>9.694594126357559</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>6178074.5</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>-0.48665440625</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>-5.222847499999999</v>
       </c>
-      <c r="K41" t="n">
+      <c r="L41" t="n">
         <v>0.3435326643593105</v>
       </c>
     </row>
@@ -2210,7 +2335,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2236,35 +2361,40 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Thickness</t>
+          <t>Designed Thickness</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Leg size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Weld type</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Weld length</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Normal stress</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Shear stress</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Shear stress 2</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Normal stress 2</t>
         </is>
@@ -2289,24 +2419,27 @@
       <c r="D2" t="n">
         <v>0.005</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
+      <c r="E2" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>-0.0894916977246423</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>-0.01097447591209279</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.04276552590891544</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>-0.01475784835819022</v>
       </c>
     </row>
@@ -2329,24 +2462,27 @@
       <c r="D3" t="n">
         <v>0.005</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="E3" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>-0.1725183344658662</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>-0.003022505470979381</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>-0.04620276320127561</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.00251378110950267</v>
       </c>
     </row>
@@ -2369,24 +2505,27 @@
       <c r="D4" t="n">
         <v>0.005</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
+      <c r="E4" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>-0.08384220284691597</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>-0.00286474826497894</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.04183817771307759</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>-0.03682890912495915</v>
       </c>
     </row>
@@ -2409,24 +2548,27 @@
       <c r="D5" t="n">
         <v>0.005</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
+      <c r="E5" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>-0.1131670918339483</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>-0.00356279819514587</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>-0.02098383037264357</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>-0.0009161947063564725</v>
       </c>
     </row>
@@ -2449,24 +2591,27 @@
       <c r="D6" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>-0.3913531880621793</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>-0.004067059678394663</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>-0.03443978311912984</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>-0.3184758957305582</v>
       </c>
     </row>
@@ -2489,24 +2634,27 @@
       <c r="D7" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>-0.3431951115657714</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>-0.0267593576352841</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.1124526404425089</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>-0.2472358311842534</v>
       </c>
     </row>
@@ -2529,25 +2677,28 @@
       <c r="D8" t="n">
         <v>0.004</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
+      <c r="E8" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>-0.1835056543101943</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>0.02219483358950252</v>
       </c>
-      <c r="I8" t="n">
-        <v>0.05829910875143682</v>
-      </c>
       <c r="J8" t="n">
-        <v>0.02643580455457226</v>
+        <v>0.05829910883094968</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.02643580465145895</v>
       </c>
     </row>
     <row r="9">
@@ -2569,24 +2720,27 @@
       <c r="D9" t="n">
         <v>0.004</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
+      <c r="E9" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>-0.08667373907856747</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>0.00059322862243952</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>-0.03987204710351332</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>-0.05950885116898916</v>
       </c>
     </row>
@@ -2609,24 +2763,27 @@
       <c r="D10" t="n">
         <v>0.005</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
+      <c r="E10" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>-9.548023014238131</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>-1.20776287443621</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>-4.568091754186073</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>-3.179268599162613</v>
       </c>
     </row>
@@ -2649,24 +2806,27 @@
       <c r="D11" t="n">
         <v>0.005</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
+      <c r="E11" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>-17.76734751790967</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>-0.2502095130060863</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>-4.075892337398034</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>-1.652065945034609</v>
       </c>
     </row>
@@ -2689,24 +2849,27 @@
       <c r="D12" t="n">
         <v>0.005</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
+      <c r="E12" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>-8.459275214159971</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>-0.236761252799257</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>4.197215673380804</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>-3.81912874874097</v>
       </c>
     </row>
@@ -2729,24 +2892,27 @@
       <c r="D13" t="n">
         <v>0.005</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
+      <c r="E13" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>11.42153896784345</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>0.2913604483171654</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>-1.73938056381853</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>-1.225767798595375</v>
       </c>
     </row>
@@ -2769,24 +2935,27 @@
       <c r="D14" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>-34.95129484712607</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>-0.3677226008000619</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>-3.099492043447932</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>-28.42193644524374</v>
       </c>
     </row>
@@ -2809,24 +2978,27 @@
       <c r="D15" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>-30.68094370944615</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>-2.366646215854448</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>10.03217950907694</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>-22.12054580397844</v>
       </c>
     </row>
@@ -2849,24 +3021,27 @@
       <c r="D16" t="n">
         <v>0.004</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
+      <c r="E16" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>-16.34836705860689</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>1.968989531568899</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>5.183674175239181</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>2.356543638233337</v>
       </c>
     </row>
@@ -2889,24 +3064,27 @@
       <c r="D17" t="n">
         <v>0.004</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
+      <c r="E17" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>-7.714972420874599</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.04961517376261602</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>-3.565387661588549</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>-5.294030168217454</v>
       </c>
     </row>
@@ -2929,24 +3107,27 @@
       <c r="D18" t="n">
         <v>0.005</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
+      <c r="E18" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>-0.2437503539082308</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>-0.03022758081884601</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.1165230469541738</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>-0.04200801582759128</v>
       </c>
     </row>
@@ -2969,24 +3150,27 @@
       <c r="D19" t="n">
         <v>0.005</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
+      <c r="E19" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>-0.4638773405422534</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>-0.007544556406044917</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>-0.1179458588485016</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>0.008927691488147586</v>
       </c>
     </row>
@@ -3009,24 +3193,27 @@
       <c r="D20" t="n">
         <v>0.005</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
+      <c r="E20" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>-0.2238690710286164</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>-0.007190741998989419</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>0.1115113987411822</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>-0.09926870730155125</v>
       </c>
     </row>
@@ -3049,24 +3236,27 @@
       <c r="D21" t="n">
         <v>0.005</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
+      <c r="E21" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>-0.300716720704968</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>-0.009243805881817784</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>-0.0525388837399569</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>-0.0355139469864517</v>
       </c>
     </row>
@@ -3089,24 +3279,27 @@
       <c r="D22" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E22" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>-1.003100630599387</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>-0.01043969161072637</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>-0.08849527671379862</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>-0.8160976682694595</v>
       </c>
     </row>
@@ -3129,24 +3322,27 @@
       <c r="D23" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E23" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F23" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>-0.8800159108804796</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>-0.06845959454689819</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>0.2881365424359664</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>-0.6341698017590369</v>
       </c>
     </row>
@@ -3169,24 +3365,27 @@
       <c r="D24" t="n">
         <v>0.004</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
+      <c r="E24" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>-0.4700194486266598</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>0.05677025400240721</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>0.1492373163352728</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>0.06771272115655412</v>
       </c>
     </row>
@@ -3209,24 +3408,27 @@
       <c r="D25" t="n">
         <v>0.004</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
+      <c r="E25" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>-0.2219811122982303</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>0.001484802011635252</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>-0.1022205482752319</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>-0.1523662250814712</v>
       </c>
     </row>
@@ -3249,25 +3451,28 @@
       <c r="D26" t="n">
         <v>0.005</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
+      <c r="E26" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>-0.4999729595108714</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>-0.06242902306127613</v>
       </c>
-      <c r="I26" t="n">
-        <v>-0.2390974718317553</v>
-      </c>
       <c r="J26" t="n">
-        <v>-0.1619009765131031</v>
+        <v>-0.2390974716996432</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-0.1619009769022927</v>
       </c>
     </row>
     <row r="27">
@@ -3289,25 +3494,28 @@
       <c r="D27" t="n">
         <v>0.005</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
+      <c r="E27" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>-0.9437666760193747</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>-0.01460206722282682</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>-0.2317962238876436</v>
       </c>
-      <c r="J27" t="n">
-        <v>0.02097400137106597</v>
+      <c r="K27" t="n">
+        <v>0.02097400149131166</v>
       </c>
     </row>
     <row r="28">
@@ -3329,24 +3537,27 @@
       <c r="D28" t="n">
         <v>0.005</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
+      <c r="E28" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>-0.4534220010351871</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>-0.01395749467430451</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>0.2255849311358745</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>-0.2022714803457344</v>
       </c>
     </row>
@@ -3369,24 +3580,27 @@
       <c r="D29" t="n">
         <v>0.005</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
+      <c r="E29" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>0.6098995020989016</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>0.01516102400605136</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>-0.1018816004497758</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>-0.06989803978510954</v>
       </c>
     </row>
@@ -3409,24 +3623,27 @@
       <c r="D30" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E30" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F30" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>-1.976837831618049</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>-0.02059496495592024</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>-0.1746985356372362</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>-1.608030966198513</v>
       </c>
     </row>
@@ -3449,24 +3666,27 @@
       <c r="D31" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E31" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>-1.734745107737569</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>-0.1347340026776136</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>0.5677013078847597</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>-1.25040076105503</v>
       </c>
     </row>
@@ -3489,24 +3709,27 @@
       <c r="D32" t="n">
         <v>0.004</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
+      <c r="E32" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>-0.9258174706278742</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>0.1117197364315765</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>0.2938408173227242</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>0.1333801388147645</v>
       </c>
     </row>
@@ -3529,24 +3752,27 @@
       <c r="D33" t="n">
         <v>0.004</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
+      <c r="E33" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>-0.4372154038207766</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>0.002879908091428529</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>-0.20148042403395</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>-0.300047849739252</v>
       </c>
     </row>
@@ -3569,24 +3795,27 @@
       <c r="D34" t="n">
         <v>0.005</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
+      <c r="E34" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>-0.7939108618347768</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>-0.09944735195119433</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>-0.3797322797838663</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>-0.2589064513454973</v>
       </c>
     </row>
@@ -3609,24 +3838,27 @@
       <c r="D35" t="n">
         <v>0.005</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
+      <c r="E35" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>-1.493084245121062</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>-0.02256976233160518</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>-0.3608232232162219</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>0.03524966611711217</v>
       </c>
     </row>
@@ -3649,25 +3881,28 @@
       <c r="D36" t="n">
         <v>0.005</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
+      <c r="E36" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>-0.7158622010738013</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>-0.02159885576484726</v>
       </c>
-      <c r="I36" t="n">
-        <v>0.3559472437636689</v>
-      </c>
       <c r="J36" t="n">
-        <v>-0.3202484667566411</v>
+        <v>0.3559472466513669</v>
+      </c>
+      <c r="K36" t="n">
+        <v>-0.3202484630707669</v>
       </c>
     </row>
     <row r="37">
@@ -3689,24 +3924,27 @@
       <c r="D37" t="n">
         <v>0.005</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
+      <c r="E37" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>0.9637591753954005</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>0.02411618805734283</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
         <v>-0.1575475722814395</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>-0.1088640923084915</v>
       </c>
     </row>
@@ -3729,24 +3967,27 @@
       <c r="D38" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E38" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F38" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>-3.081250956615169</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>-0.03212237050523915</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>-0.272521525445181</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>-2.506196475414759</v>
       </c>
     </row>
@@ -3769,24 +4010,27 @@
       <c r="D39" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E39" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F39" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>-2.70424668402679</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>-0.2098553033395461</v>
       </c>
-      <c r="I39" t="n">
+      <c r="J39" t="n">
         <v>0.8847614396036747</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>-1.949419649591241</v>
       </c>
     </row>
@@ -3809,24 +4053,27 @@
       <c r="D40" t="n">
         <v>0.004</v>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
+      <c r="E40" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>-1.44269890027788</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>0.1740148017675522</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>0.4578016870625739</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>0.2078506277226174</v>
       </c>
     </row>
@@ -3849,24 +4096,27 @@
       <c r="D41" t="n">
         <v>0.004</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
+      <c r="E41" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>-0.6812808682840974</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>0.004454344342679258</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>-0.3140702378611531</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>-0.4675046645192003</v>
       </c>
     </row>
@@ -3889,24 +4139,27 @@
       <c r="D42" t="n">
         <v>0.005</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
+      <c r="E42" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>-1.335139178312906</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>-0.167850027976392</v>
       </c>
-      <c r="I42" t="n">
+      <c r="J42" t="n">
         <v>-0.6387330538737687</v>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>-0.4387503442492822</v>
       </c>
     </row>
@@ -3929,24 +4182,27 @@
       <c r="D43" t="n">
         <v>0.005</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
+      <c r="E43" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>-2.500707233086861</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>-0.03683855481803039</v>
       </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
         <v>-0.5934124350703039</v>
       </c>
-      <c r="J43" t="n">
+      <c r="K43" t="n">
         <v>0.06294948017473591</v>
       </c>
     </row>
@@ -3969,24 +4225,27 @@
       <c r="D44" t="n">
         <v>0.005</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
+      <c r="E44" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>-1.19624485792061</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>-0.03528599820568968</v>
       </c>
-      <c r="I44" t="n">
+      <c r="J44" t="n">
         <v>0.594396828771124</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>-0.5368868542205741</v>
       </c>
     </row>
@@ -4009,25 +4268,28 @@
       <c r="D45" t="n">
         <v>0.005</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
+      <c r="E45" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>1.612085730849879</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>0.04062943220087874</v>
       </c>
-      <c r="I45" t="n">
+      <c r="J45" t="n">
         <v>-0.2570771714683082</v>
       </c>
-      <c r="J45" t="n">
-        <v>-0.179112321792917</v>
+      <c r="K45" t="n">
+        <v>-0.1791123169174473</v>
       </c>
     </row>
     <row r="46">
@@ -4049,24 +4311,27 @@
       <c r="D46" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E46" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F46" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>-5.074857725247503</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>-0.05295634803149062</v>
       </c>
-      <c r="I46" t="n">
+      <c r="J46" t="n">
         <v>-0.4492666662459144</v>
       </c>
-      <c r="J46" t="n">
+      <c r="K46" t="n">
         <v>-4.127354085767516</v>
       </c>
     </row>
@@ -4089,24 +4354,27 @@
       <c r="D47" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E47" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F47" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>-4.454543657206472</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>-0.3453189166051464</v>
       </c>
-      <c r="I47" t="n">
+      <c r="J47" t="n">
         <v>1.457022006525985</v>
       </c>
-      <c r="J47" t="n">
+      <c r="K47" t="n">
         <v>-3.211533570437346</v>
       </c>
     </row>
@@ -4129,24 +4397,27 @@
       <c r="D48" t="n">
         <v>0.004</v>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F48" t="n">
+      <c r="E48" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>-2.375467780810389</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>0.2863760178642489</v>
       </c>
-      <c r="I48" t="n">
+      <c r="J48" t="n">
         <v>0.7536189903536468</v>
       </c>
-      <c r="J48" t="n">
+      <c r="K48" t="n">
         <v>0.3422480628275607</v>
       </c>
     </row>
@@ -4169,24 +4440,27 @@
       <c r="D49" t="n">
         <v>0.004</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F49" t="n">
+      <c r="E49" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>-1.121685920035047</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>0.007271991544192271</v>
       </c>
-      <c r="I49" t="n">
+      <c r="J49" t="n">
         <v>-0.51733610774662</v>
       </c>
-      <c r="J49" t="n">
+      <c r="K49" t="n">
         <v>-0.7696500489065223</v>
       </c>
     </row>
@@ -4209,24 +4483,27 @@
       <c r="D50" t="n">
         <v>0.005</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F50" t="n">
+      <c r="E50" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>-2.168203126465291</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>-0.2733122815653218</v>
       </c>
-      <c r="I50" t="n">
+      <c r="J50" t="n">
         <v>-1.037356780784754</v>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>-0.7164820886373848</v>
       </c>
     </row>
@@ -4249,24 +4526,27 @@
       <c r="D51" t="n">
         <v>0.005</v>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F51" t="n">
+      <c r="E51" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>-4.048915472936102</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>-0.05849173709102842</v>
       </c>
-      <c r="I51" t="n">
+      <c r="J51" t="n">
         <v>-0.9476181870827846</v>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>0.1067872073739555</v>
       </c>
     </row>
@@ -4289,24 +4569,27 @@
       <c r="D52" t="n">
         <v>0.005</v>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F52" t="n">
+      <c r="E52" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>-1.933490840680957</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>-0.05601318470887048</v>
       </c>
-      <c r="I52" t="n">
+      <c r="J52" t="n">
         <v>0.9602090139062135</v>
       </c>
-      <c r="J52" t="n">
+      <c r="K52" t="n">
         <v>-0.8698579654372541</v>
       </c>
     </row>
@@ -4329,24 +4612,27 @@
       <c r="D53" t="n">
         <v>0.005</v>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F53" t="n">
+      <c r="E53" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>2.607559040809714</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>0.06607311708264435</v>
       </c>
-      <c r="I53" t="n">
+      <c r="J53" t="n">
         <v>-0.4080360013352027</v>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>-0.2860500786029579</v>
       </c>
     </row>
@@ -4369,24 +4655,27 @@
       <c r="D54" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E54" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F54" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G54" t="n">
+      <c r="H54" t="n">
         <v>-8.113126441065321</v>
       </c>
-      <c r="H54" t="n">
+      <c r="I54" t="n">
         <v>-0.08475376839597297</v>
       </c>
-      <c r="I54" t="n">
+      <c r="J54" t="n">
         <v>-0.718751691421384</v>
       </c>
-      <c r="J54" t="n">
+      <c r="K54" t="n">
         <v>-6.597911056974861</v>
       </c>
     </row>
@@ -4409,24 +4698,27 @@
       <c r="D55" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E55" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F55" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>-7.12210925605882</v>
       </c>
-      <c r="H55" t="n">
+      <c r="I55" t="n">
         <v>-0.5515682406855026</v>
       </c>
-      <c r="I55" t="n">
+      <c r="J55" t="n">
         <v>2.329091293147588</v>
       </c>
-      <c r="J55" t="n">
+      <c r="K55" t="n">
         <v>-5.135132923586928</v>
       </c>
     </row>
@@ -4449,24 +4741,27 @@
       <c r="D56" t="n">
         <v>0.004</v>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F56" t="n">
+      <c r="E56" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>-3.796768387561857</v>
       </c>
-      <c r="H56" t="n">
+      <c r="I56" t="n">
         <v>0.4575419837731778</v>
       </c>
-      <c r="I56" t="n">
+      <c r="J56" t="n">
         <v>1.20430861889481</v>
       </c>
-      <c r="J56" t="n">
+      <c r="K56" t="n">
         <v>0.5470522079382574</v>
       </c>
     </row>
@@ -4489,24 +4784,27 @@
       <c r="D57" t="n">
         <v>0.004</v>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F57" t="n">
+      <c r="E57" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>-1.792678910229334</v>
       </c>
-      <c r="H57" t="n">
+      <c r="I57" t="n">
         <v>0.01155282272932846</v>
       </c>
-      <c r="I57" t="n">
+      <c r="J57" t="n">
         <v>-0.8271540596485909</v>
       </c>
-      <c r="J57" t="n">
+      <c r="K57" t="n">
         <v>-1.229989536350789</v>
       </c>
     </row>
@@ -4529,24 +4827,27 @@
       <c r="D58" t="n">
         <v>0.005</v>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F58" t="n">
+      <c r="E58" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>-3.046638757046086</v>
       </c>
-      <c r="H58" t="n">
+      <c r="I58" t="n">
         <v>-0.3846452416722271</v>
       </c>
-      <c r="I58" t="n">
+      <c r="J58" t="n">
         <v>-1.457687823659216</v>
       </c>
-      <c r="J58" t="n">
+      <c r="K58" t="n">
         <v>-1.010015244909688</v>
       </c>
     </row>
@@ -4569,24 +4870,27 @@
       <c r="D59" t="n">
         <v>0.005</v>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F59" t="n">
+      <c r="E59" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>-5.679587971160125</v>
       </c>
-      <c r="H59" t="n">
+      <c r="I59" t="n">
         <v>-0.0811162496816311</v>
       </c>
-      <c r="I59" t="n">
+      <c r="J59" t="n">
         <v>-1.318391858075389</v>
       </c>
-      <c r="J59" t="n">
+      <c r="K59" t="n">
         <v>0.1539880096185585</v>
       </c>
     </row>
@@ -4609,24 +4913,27 @@
       <c r="D60" t="n">
         <v>0.005</v>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F60" t="n">
+      <c r="E60" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G60" t="n">
+      <c r="H60" t="n">
         <v>-2.709317381340957</v>
       </c>
-      <c r="H60" t="n">
+      <c r="I60" t="n">
         <v>-0.07759717151622363</v>
       </c>
-      <c r="I60" t="n">
+      <c r="J60" t="n">
         <v>1.345089410504968</v>
       </c>
-      <c r="J60" t="n">
+      <c r="K60" t="n">
         <v>-1.220635077866374</v>
       </c>
     </row>
@@ -4649,24 +4956,27 @@
       <c r="D61" t="n">
         <v>0.005</v>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F61" t="n">
+      <c r="E61" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>3.655516485015514</v>
       </c>
-      <c r="H61" t="n">
+      <c r="I61" t="n">
         <v>0.09290788558102335</v>
       </c>
-      <c r="I61" t="n">
+      <c r="J61" t="n">
         <v>-0.5656099760801708</v>
       </c>
-      <c r="J61" t="n">
+      <c r="K61" t="n">
         <v>-0.3979059545060382</v>
       </c>
     </row>
@@ -4689,24 +4999,27 @@
       <c r="D62" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E62" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F62" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>-11.29508844321172</v>
       </c>
-      <c r="H62" t="n">
+      <c r="I62" t="n">
         <v>-0.1181096419895265</v>
       </c>
-      <c r="I62" t="n">
+      <c r="J62" t="n">
         <v>-1.00106998165407</v>
       </c>
-      <c r="J62" t="n">
+      <c r="K62" t="n">
         <v>-9.1852548959363</v>
       </c>
     </row>
@@ -4729,24 +5042,27 @@
       <c r="D63" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E63" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F63" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>-9.915852858981724</v>
       </c>
-      <c r="H63" t="n">
+      <c r="I63" t="n">
         <v>-0.7673592041004744</v>
       </c>
-      <c r="I63" t="n">
+      <c r="J63" t="n">
         <v>3.242358455233986</v>
       </c>
-      <c r="J63" t="n">
+      <c r="K63" t="n">
         <v>-7.149725828913328</v>
       </c>
     </row>
@@ -4769,24 +5085,27 @@
       <c r="D64" t="n">
         <v>0.004</v>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F64" t="n">
+      <c r="E64" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>-5.285080000566125</v>
       </c>
-      <c r="H64" t="n">
+      <c r="I64" t="n">
         <v>0.6367485180246486</v>
       </c>
-      <c r="I64" t="n">
+      <c r="J64" t="n">
         <v>1.676197295813028</v>
       </c>
-      <c r="J64" t="n">
+      <c r="K64" t="n">
         <v>0.7615338752623041</v>
       </c>
     </row>
@@ -4809,24 +5128,27 @@
       <c r="D65" t="n">
         <v>0.004</v>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F65" t="n">
+      <c r="E65" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>-2.495220281007457</v>
       </c>
-      <c r="H65" t="n">
+      <c r="I65" t="n">
         <v>0.01603089296027076</v>
       </c>
-      <c r="I65" t="n">
+      <c r="J65" t="n">
         <v>-1.151668922450829</v>
       </c>
-      <c r="J65" t="n">
+      <c r="K65" t="n">
         <v>-1.711984278509386</v>
       </c>
     </row>
@@ -4849,24 +5171,27 @@
       <c r="D66" t="n">
         <v>0.005</v>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F66" t="n">
+      <c r="E66" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G66" t="n">
+      <c r="H66" t="n">
         <v>-3.978458102506766</v>
       </c>
-      <c r="H66" t="n">
+      <c r="I66" t="n">
         <v>-0.5027799768619037</v>
       </c>
-      <c r="I66" t="n">
+      <c r="J66" t="n">
         <v>-1.903561632365459</v>
       </c>
-      <c r="J66" t="n">
+      <c r="K66" t="n">
         <v>-1.321690745279651</v>
       </c>
     </row>
@@ -4889,24 +5214,27 @@
       <c r="D67" t="n">
         <v>0.005</v>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F67" t="n">
+      <c r="E67" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G67" t="n">
+      <c r="H67" t="n">
         <v>-7.408756399203434</v>
       </c>
-      <c r="H67" t="n">
+      <c r="I67" t="n">
         <v>-0.1050344548814284</v>
       </c>
-      <c r="I67" t="n">
+      <c r="J67" t="n">
         <v>-1.710501706304018</v>
       </c>
-      <c r="J67" t="n">
+      <c r="K67" t="n">
         <v>0.204689841166334</v>
       </c>
     </row>
@@ -4929,24 +5257,27 @@
       <c r="D68" t="n">
         <v>0.005</v>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F68" t="n">
+      <c r="E68" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G68" t="n">
+      <c r="H68" t="n">
         <v>-3.531628207409936</v>
       </c>
-      <c r="H68" t="n">
+      <c r="I68" t="n">
         <v>-0.100345277881468</v>
       </c>
-      <c r="I68" t="n">
+      <c r="J68" t="n">
         <v>1.752978713447105</v>
       </c>
-      <c r="J68" t="n">
+      <c r="K68" t="n">
         <v>-1.592612605246398</v>
       </c>
     </row>
@@ -4969,24 +5300,27 @@
       <c r="D69" t="n">
         <v>0.005</v>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F69" t="n">
+      <c r="E69" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G69" t="n">
+      <c r="H69" t="n">
         <v>4.766443323587651</v>
       </c>
-      <c r="H69" t="n">
+      <c r="I69" t="n">
         <v>0.1213738568850457</v>
       </c>
-      <c r="I69" t="n">
+      <c r="J69" t="n">
         <v>-0.7320475570038235</v>
       </c>
-      <c r="J69" t="n">
+      <c r="K69" t="n">
         <v>-0.5160724824154229</v>
       </c>
     </row>
@@ -5009,24 +5343,27 @@
       <c r="D70" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="E70" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F70" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G70" t="n">
+      <c r="H70" t="n">
         <v>-14.66087281815081</v>
       </c>
-      <c r="H70" t="n">
+      <c r="I70" t="n">
         <v>-0.1534525850643296</v>
       </c>
-      <c r="I70" t="n">
+      <c r="J70" t="n">
         <v>-1.299738373338525</v>
       </c>
-      <c r="J70" t="n">
+      <c r="K70" t="n">
         <v>-11.92205774623356</v>
       </c>
     </row>
@@ -5049,24 +5386,27 @@
       <c r="D71" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E71" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F71" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G71" t="n">
+      <c r="H71" t="n">
         <v>-12.8709134990931</v>
       </c>
-      <c r="H71" t="n">
+      <c r="I71" t="n">
         <v>-0.9954126923464988</v>
       </c>
-      <c r="I71" t="n">
+      <c r="J71" t="n">
         <v>4.208365270627211</v>
       </c>
-      <c r="J71" t="n">
+      <c r="K71" t="n">
         <v>-9.28059375105911</v>
       </c>
     </row>
@@ -5089,24 +5429,27 @@
       <c r="D72" t="n">
         <v>0.004</v>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F72" t="n">
+      <c r="E72" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G72" t="n">
+      <c r="H72" t="n">
         <v>-6.859233312941224</v>
       </c>
-      <c r="H72" t="n">
+      <c r="I72" t="n">
         <v>0.8262755085218303</v>
       </c>
-      <c r="I72" t="n">
+      <c r="J72" t="n">
         <v>2.175271503366397</v>
       </c>
-      <c r="J72" t="n">
+      <c r="K72" t="n">
         <v>0.9884097783024584</v>
       </c>
     </row>
@@ -5129,24 +5472,27 @@
       <c r="D73" t="n">
         <v>0.004</v>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F73" t="n">
+      <c r="E73" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G73" t="n">
+      <c r="H73" t="n">
         <v>-3.238189564523928</v>
       </c>
-      <c r="H73" t="n">
+      <c r="I73" t="n">
         <v>0.02076810419767001</v>
       </c>
-      <c r="I73" t="n">
+      <c r="J73" t="n">
         <v>-1.494975597996788</v>
       </c>
-      <c r="J73" t="n">
+      <c r="K73" t="n">
         <v>-2.221736619420154</v>
       </c>
     </row>
@@ -5169,24 +5515,27 @@
       <c r="D74" t="n">
         <v>0.005</v>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F74" t="n">
+      <c r="E74" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G74" t="n">
+      <c r="H74" t="n">
         <v>-5.884265864975088</v>
       </c>
-      <c r="H74" t="n">
+      <c r="I74" t="n">
         <v>-0.744039870090954</v>
       </c>
-      <c r="I74" t="n">
+      <c r="J74" t="n">
         <v>-2.815390934050011</v>
       </c>
-      <c r="J74" t="n">
+      <c r="K74" t="n">
         <v>-1.95733662111151</v>
       </c>
     </row>
@@ -5209,24 +5558,27 @@
       <c r="D75" t="n">
         <v>0.005</v>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F75" t="n">
+      <c r="E75" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
         <v>0.5330616740578964</v>
       </c>
-      <c r="G75" t="n">
+      <c r="H75" t="n">
         <v>-10.95199643456471</v>
       </c>
-      <c r="H75" t="n">
+      <c r="I75" t="n">
         <v>-0.1546174097693317</v>
       </c>
-      <c r="I75" t="n">
+      <c r="J75" t="n">
         <v>-2.519784445878237</v>
       </c>
-      <c r="J75" t="n">
+      <c r="K75" t="n">
         <v>0.3074726512930047</v>
       </c>
     </row>
@@ -5249,24 +5601,27 @@
       <c r="D76" t="n">
         <v>0.005</v>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F76" t="n">
+      <c r="E76" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G76" t="n">
+      <c r="H76" t="n">
         <v>-5.217701650897061</v>
       </c>
-      <c r="H76" t="n">
+      <c r="I76" t="n">
         <v>-0.1472578061408481</v>
       </c>
-      <c r="I76" t="n">
+      <c r="J76" t="n">
         <v>2.589427531871292</v>
       </c>
-      <c r="J76" t="n">
+      <c r="K76" t="n">
         <v>-2.354401562314329</v>
       </c>
     </row>
@@ -5289,24 +5644,27 @@
       <c r="D77" t="n">
         <v>0.005</v>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F77" t="n">
+      <c r="E77" t="n">
+        <v>0.007071067811865476</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
         <v>0.568910344530199</v>
       </c>
-      <c r="G77" t="n">
+      <c r="H77" t="n">
         <v>7.043480995546354</v>
       </c>
-      <c r="H77" t="n">
+      <c r="I77" t="n">
         <v>0.1795569281824164</v>
       </c>
-      <c r="I77" t="n">
+      <c r="J77" t="n">
         <v>-1.076727872016861</v>
       </c>
-      <c r="J77" t="n">
+      <c r="K77" t="n">
         <v>-0.7594461486918507</v>
       </c>
     </row>
@@ -5329,24 +5687,27 @@
       <c r="D78" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="E78" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F78" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>0.545014923856265</v>
       </c>
-      <c r="G78" t="n">
+      <c r="H78" t="n">
         <v>-21.60334774814882</v>
       </c>
-      <c r="H78" t="n">
+      <c r="I78" t="n">
         <v>-0.2265287288748662</v>
       </c>
-      <c r="I78" t="n">
+      <c r="J78" t="n">
         <v>-1.915543136015479</v>
       </c>
-      <c r="J78" t="n">
+      <c r="K78" t="n">
         <v>-17.56745862142131</v>
       </c>
     </row>
@@ -5369,24 +5730,27 @@
       <c r="D79" t="n">
         <v>0.005656854249492381</v>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="E79" t="n">
+        <v>0.008000000000000002</v>
+      </c>
+      <c r="F79" t="inlineStr">
         <is>
           <t>pjpRear</t>
         </is>
       </c>
-      <c r="F79" t="n">
+      <c r="G79" t="n">
         <v>0.6282384253699658</v>
       </c>
-      <c r="G79" t="n">
+      <c r="H79" t="n">
         <v>-18.96532240205086</v>
       </c>
-      <c r="H79" t="n">
+      <c r="I79" t="n">
         <v>-1.465348968654687</v>
       </c>
-      <c r="I79" t="n">
+      <c r="J79" t="n">
         <v>6.201025650938556</v>
       </c>
-      <c r="J79" t="n">
+      <c r="K79" t="n">
         <v>-13.67468381519331</v>
       </c>
     </row>
@@ -5409,24 +5773,27 @@
       <c r="D80" t="n">
         <v>0.004</v>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F80" t="n">
+      <c r="E80" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G80" t="n">
+      <c r="H80" t="n">
         <v>-10.10631090781625</v>
       </c>
-      <c r="H80" t="n">
+      <c r="I80" t="n">
         <v>1.217298201167107</v>
       </c>
-      <c r="I80" t="n">
+      <c r="J80" t="n">
         <v>3.204779716749733</v>
       </c>
-      <c r="J80" t="n">
+      <c r="K80" t="n">
         <v>1.456472210269803</v>
       </c>
     </row>
@@ -5449,24 +5816,27 @@
       <c r="D81" t="n">
         <v>0.004</v>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>filletRear</t>
-        </is>
-      </c>
-      <c r="F81" t="n">
+      <c r="E81" t="n">
+        <v>0.005656854249492381</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>filletRear</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
         <v>1.016427811973747</v>
       </c>
-      <c r="G81" t="n">
+      <c r="H81" t="n">
         <v>-4.77047231901711</v>
       </c>
-      <c r="H81" t="n">
+      <c r="I81" t="n">
         <v>0.03060128933266679</v>
       </c>
-      <c r="I81" t="n">
+      <c r="J81" t="n">
         <v>-2.203209475538625</v>
       </c>
-      <c r="J81" t="n">
+      <c r="K81" t="n">
         <v>-3.273173705008115</v>
       </c>
     </row>

</xml_diff>